<commit_message>
edits to attribute tables
</commit_message>
<xml_diff>
--- a/eims-toi-transect/RaEn617withbiosat.xlsx
+++ b/eims-toi-transect/RaEn617withbiosat.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaxinewolfe/Documents/WHOI/NESLTER/nes-lter-eims-toi-ncp-gop/eims-toi-transect/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA7D5C3-16AE-9D4F-A5B8-D8915F319805}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDBE5077-D47F-FC41-B2EF-1CB526AD2937}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" xr2:uid="{C982A258-9431-4047-A26D-7AA9D305FC15}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
   <si>
     <t>attributeName</t>
   </si>
@@ -78,18 +78,12 @@
     <t>dimensionless</t>
   </si>
   <si>
-    <t>lat</t>
-  </si>
-  <si>
     <t>Latitude of sample event</t>
   </si>
   <si>
     <t>degree</t>
   </si>
   <si>
-    <t>lon</t>
-  </si>
-  <si>
     <t>Longitude of sample event</t>
   </si>
   <si>
@@ -117,13 +111,28 @@
     <t>Salinity of sampling in PSU</t>
   </si>
   <si>
-    <t>O2_Ar_ratio</t>
-  </si>
-  <si>
-    <t>Oxygen-argon ratio of underway sample corrected for air values</t>
-  </si>
-  <si>
     <t xml:space="preserve">Percent biological saturation, the oxygen-argon ratio divided by the equilibrium value of that ratio </t>
+  </si>
+  <si>
+    <t>O2_Ar_ratio_corrected</t>
+  </si>
+  <si>
+    <t>latitude</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>Oxygen-argon ratio of EIMS sample from underway corrected for air values</t>
+  </si>
+  <si>
+    <t>depth</t>
+  </si>
+  <si>
+    <t>Depth of sample below sea surface. URI http://vocab.nerc.ac.uk/collection/P09/current/DEPH/</t>
+  </si>
+  <si>
+    <t>meter</t>
   </si>
 </sst>
 </file>
@@ -478,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCDD1288-8881-B24F-9A15-6CAF4EADEF4D}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A6" sqref="A6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -543,78 +552,72 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
         <v>16</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C5" t="s">
         <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
         <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" t="s">
         <v>23</v>
       </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" t="s">
-        <v>25</v>
-      </c>
       <c r="G7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
@@ -623,18 +626,18 @@
         <v>14</v>
       </c>
       <c r="F8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
         <v>13</v>
@@ -643,10 +646,30 @@
         <v>14</v>
       </c>
       <c r="F9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G9" t="s">
-        <v>26</v>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated depth and datetime column names
</commit_message>
<xml_diff>
--- a/eims-toi-transect/RaEn617withbiosat.xlsx
+++ b/eims-toi-transect/RaEn617withbiosat.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaxinewolfe/Documents/WHOI/NESLTER/nes-lter-eims-toi-ncp-gop/eims-toi-transect/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wanglab\Documents\GitHub\nes-lter-eims-toi-ncp-gop\eims-toi-transect\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDBE5077-D47F-FC41-B2EF-1CB526AD2937}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" xr2:uid="{C982A258-9431-4047-A26D-7AA9D305FC15}"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14580"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -54,9 +53,6 @@
     <t>missingValueCodeExplanation</t>
   </si>
   <si>
-    <t>utc_datetime</t>
-  </si>
-  <si>
     <t>Date and time in UTC</t>
   </si>
   <si>
@@ -66,9 +62,6 @@
     <t>YYYY-MM-DD hh:mm:ss</t>
   </si>
   <si>
-    <t>matlab_datetime</t>
-  </si>
-  <si>
     <t>UTC date and time in MATLAB serial date number format</t>
   </si>
   <si>
@@ -133,12 +126,18 @@
   </si>
   <si>
     <t>meter</t>
+  </si>
+  <si>
+    <t>datetime_utc</t>
+  </si>
+  <si>
+    <t>datetime_utc_matlab</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -486,20 +485,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FCDD1288-8881-B24F-9A15-6CAF4EADEF4D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:D6"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="76.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="76.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -522,154 +521,154 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
         <v>28</v>
       </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" t="s">
-        <v>32</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" t="s">
-        <v>23</v>
-      </c>
-      <c r="G7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" t="s">
         <v>21</v>
       </c>
-      <c r="B8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="G10" t="s">
         <v>22</v>
-      </c>
-      <c r="B9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" t="s">
-        <v>13</v>
-      </c>
-      <c r="D9" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
temp & sal not provided in RaEn617withbiosat.csv
</commit_message>
<xml_diff>
--- a/eims-toi-transect/RaEn617withbiosat.xlsx
+++ b/eims-toi-transect/RaEn617withbiosat.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t>attributeName</t>
   </si>
@@ -80,18 +80,6 @@
     <t>Longitude of sample event</t>
   </si>
   <si>
-    <t>temp</t>
-  </si>
-  <si>
-    <t>Temperature of sampling</t>
-  </si>
-  <si>
-    <t>celsius</t>
-  </si>
-  <si>
-    <t>sal</t>
-  </si>
-  <si>
     <t>biosat</t>
   </si>
   <si>
@@ -99,9 +87,6 @@
   </si>
   <si>
     <t>Missing value</t>
-  </si>
-  <si>
-    <t>Salinity of sampling in PSU</t>
   </si>
   <si>
     <t xml:space="preserve">Percent biological saturation, the oxygen-argon ratio divided by the equilibrium value of that ratio </t>
@@ -486,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A7" sqref="A7:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -523,7 +508,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -537,7 +522,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -551,7 +536,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
@@ -565,7 +550,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
@@ -579,16 +564,16 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -596,24 +581,24 @@
         <v>16</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
         <v>11</v>
       </c>
       <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" t="s">
         <v>18</v>
-      </c>
-      <c r="F7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
         <v>23</v>
@@ -625,50 +610,10 @@
         <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="G8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" t="s">
-        <v>12</v>
-      </c>
-      <c r="F9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F10" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated parameter names and units
</commit_message>
<xml_diff>
--- a/eims-toi-transect/RaEn617withbiosat.xlsx
+++ b/eims-toi-transect/RaEn617withbiosat.xlsx
@@ -92,9 +92,6 @@
     <t xml:space="preserve">Percent biological saturation, the oxygen-argon ratio divided by the equilibrium value of that ratio </t>
   </si>
   <si>
-    <t>O2_Ar_ratio_corrected</t>
-  </si>
-  <si>
     <t>latitude</t>
   </si>
   <si>
@@ -117,6 +114,9 @@
   </si>
   <si>
     <t>datetime_utc_matlab</t>
+  </si>
+  <si>
+    <t>O2_Ar_ratio</t>
   </si>
 </sst>
 </file>
@@ -474,7 +474,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -508,7 +508,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -522,7 +522,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -536,7 +536,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
@@ -550,7 +550,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
         <v>15</v>
@@ -564,16 +564,16 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
         <v>24</v>
-      </c>
-      <c r="B6" t="s">
-        <v>25</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -598,10 +598,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>

</xml_diff>